<commit_message>
addition of one more line
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810084E0-1A66-43E0-B038-74BB5F17558E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8F2EE5-B24E-4947-B986-462F18DF7EAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
   <si>
     <t>Modules</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t xml:space="preserve">Demo </t>
+  </si>
+  <si>
+    <t>Demo1</t>
   </si>
 </sst>
 </file>
@@ -786,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1463,21 +1466,17 @@
         <v>119</v>
       </c>
     </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D114" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2B1AF173142ED479DDCDE33FBDC472F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5645c10f453ab806e730b5a744b5b25f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="242e5788-3325-4b0c-8142-6fd49a4618f2" xmlns:ns3="ee8edb94-d01c-4a80-94b8-3bab0e1306d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="701c25491dcd6e28280494419172c20c" ns2:_="" ns3:_="">
     <xsd:import namespace="242e5788-3325-4b0c-8142-6fd49a4618f2"/>
@@ -1688,6 +1687,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1695,14 +1703,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95A28F03-6566-4913-9978-AC16D2197243}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8674C2BF-1067-418C-BF61-94184669BBC1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1721,6 +1721,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95A28F03-6566-4913-9978-AC16D2197243}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E19C1E25-23C7-441C-8852-7CEE76DA512D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Revert "addition of one more line"
This reverts commit 6bc888ab179b454bc98600154b4c25f71ce3c408.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8F2EE5-B24E-4947-B986-462F18DF7EAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810084E0-1A66-43E0-B038-74BB5F17558E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="120">
   <si>
     <t>Modules</t>
   </si>
@@ -391,9 +391,6 @@
   </si>
   <si>
     <t xml:space="preserve">Demo </t>
-  </si>
-  <si>
-    <t>Demo1</t>
   </si>
 </sst>
 </file>
@@ -789,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1466,17 +1463,21 @@
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D114" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2B1AF173142ED479DDCDE33FBDC472F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5645c10f453ab806e730b5a744b5b25f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="242e5788-3325-4b0c-8142-6fd49a4618f2" xmlns:ns3="ee8edb94-d01c-4a80-94b8-3bab0e1306d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="701c25491dcd6e28280494419172c20c" ns2:_="" ns3:_="">
     <xsd:import namespace="242e5788-3325-4b0c-8142-6fd49a4618f2"/>
@@ -1687,15 +1688,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1703,6 +1695,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95A28F03-6566-4913-9978-AC16D2197243}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8674C2BF-1067-418C-BF61-94184669BBC1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1721,14 +1721,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95A28F03-6566-4913-9978-AC16D2197243}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E19C1E25-23C7-441C-8852-7CEE76DA512D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
added my name for testing
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24603"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="274" documentId="11_ADDB425A97A2B533DD8E8AB2B57390742C73FC52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87CD805F-8BA0-4CF7-9DEB-32A7EC5D7261}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git clone demo2\Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CC63CA-7AFA-4F06-B2E4-8BE6602656FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="120">
   <si>
     <t>Modules</t>
   </si>
@@ -383,13 +388,16 @@
   </si>
   <si>
     <t>Verify that we should navigate back to admin homepage after changing the password.</t>
+  </si>
+  <si>
+    <t>shivam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -778,23 +786,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="89.28515625" customWidth="1"/>
+    <col min="2" max="3" width="28.81640625" customWidth="1"/>
+    <col min="4" max="4" width="89.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -805,7 +813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -819,7 +827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -828,7 +836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -837,96 +845,96 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16.5">
+    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16.5">
+    <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16.5">
+    <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -940,30 +948,30 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>3</v>
       </c>
@@ -977,50 +985,50 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.5">
+    <row r="26" spans="1:4" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.5">
+    <row r="30" spans="1:4" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>34</v>
       </c>
@@ -1031,7 +1039,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="16.5">
+    <row r="34" spans="2:5" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>37</v>
@@ -1040,14 +1048,14 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="4" t="s">
@@ -1057,14 +1065,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="16.5">
+    <row r="37" spans="2:5" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="4" t="s">
@@ -1074,28 +1082,28 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="16.5">
+    <row r="39" spans="2:5" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C42" s="1"/>
       <c r="D42" s="4" t="s">
         <v>48</v>
@@ -1104,7 +1112,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="2:5">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="4" t="s">
@@ -1114,11 +1122,11 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="2:5">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:5">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
         <v>52</v>
       </c>
@@ -1129,14 +1137,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="2:5">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="2:5">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="4" t="s">
@@ -1146,48 +1154,48 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="2:5">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="2:4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="2:4">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="2:4">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="2:4">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="2:4">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:4">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:4">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B55" s="1" t="s">
         <v>63</v>
       </c>
@@ -1198,22 +1206,22 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="2:4">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D56" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="2:4">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D57" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="2:4">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D58" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="2:4">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C60" s="6" t="s">
         <v>69</v>
       </c>
@@ -1221,22 +1229,22 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="2:4">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D61" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="2:4">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D62" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="2:4">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D63" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="3:4">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C65" t="s">
         <v>74</v>
       </c>
@@ -1244,17 +1252,17 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="3:4">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D66" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="3:4">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D67" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="3:4">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C69" t="s">
         <v>78</v>
       </c>
@@ -1262,22 +1270,22 @@
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="3:4">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D70" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="3:4">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D71" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="3:4">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D72" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="3:4">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C74" t="s">
         <v>83</v>
       </c>
@@ -1285,27 +1293,27 @@
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="3:4">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D75" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="3:4">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D76" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="3:4">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D77" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="78" spans="3:4">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D78" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="2:4">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B81" s="1" t="s">
         <v>89</v>
       </c>
@@ -1316,32 +1324,32 @@
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="2:4">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D82" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="83" spans="2:4">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D83" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="84" spans="2:4">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D84" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="2:4">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D85" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="2:4">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D86" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="88" spans="2:4">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C88" t="s">
         <v>97</v>
       </c>
@@ -1349,37 +1357,37 @@
         <v>98</v>
       </c>
     </row>
-    <row r="89" spans="2:4">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D89" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="90" spans="2:4">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D90" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="2:4">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D91" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="2:4">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D92" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="2:4">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D93" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="2:4">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D94" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="97" spans="3:4">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C97" t="s">
         <v>105</v>
       </c>
@@ -1387,42 +1395,42 @@
         <v>106</v>
       </c>
     </row>
-    <row r="98" spans="3:4">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D98" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="99" spans="3:4">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D99" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="100" spans="3:4">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D100" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="101" spans="3:4">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D101" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="102" spans="3:4">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D102" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="103" spans="3:4">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D103" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="104" spans="3:4">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D104" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="106" spans="3:4">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C106" t="s">
         <v>113</v>
       </c>
@@ -1430,24 +1438,29 @@
         <v>114</v>
       </c>
     </row>
-    <row r="107" spans="3:4">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D107" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="108" spans="3:4">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D108" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="109" spans="3:4">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D109" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="110" spans="3:4">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D110" s="7" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D115" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1456,6 +1469,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2B1AF173142ED479DDCDE33FBDC472F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5645c10f453ab806e730b5a744b5b25f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="242e5788-3325-4b0c-8142-6fd49a4618f2" xmlns:ns3="ee8edb94-d01c-4a80-94b8-3bab0e1306d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="701c25491dcd6e28280494419172c20c" ns2:_="" ns3:_="">
     <xsd:import namespace="242e5788-3325-4b0c-8142-6fd49a4618f2"/>
@@ -1666,15 +1688,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1682,13 +1695,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8674C2BF-1067-418C-BF61-94184669BBC1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95A28F03-6566-4913-9978-AC16D2197243}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95A28F03-6566-4913-9978-AC16D2197243}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8674C2BF-1067-418C-BF61-94184669BBC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="242e5788-3325-4b0c-8142-6fd49a4618f2"/>
+    <ds:schemaRef ds:uri="ee8edb94-d01c-4a80-94b8-3bab0e1306d2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E19C1E25-23C7-441C-8852-7CEE76DA512D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E19C1E25-23C7-441C-8852-7CEE76DA512D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated the same line
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git clone demo2\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CC63CA-7AFA-4F06-B2E4-8BE6602656FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB87288-D024-4EAE-8CCC-D54741D8C5D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -390,7 +390,7 @@
     <t>Verify that we should navigate back to admin homepage after changing the password.</t>
   </si>
   <si>
-    <t>shivam</t>
+    <t>shivam kushwaha</t>
   </si>
 </sst>
 </file>
@@ -1469,15 +1469,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2B1AF173142ED479DDCDE33FBDC472F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5645c10f453ab806e730b5a744b5b25f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="242e5788-3325-4b0c-8142-6fd49a4618f2" xmlns:ns3="ee8edb94-d01c-4a80-94b8-3bab0e1306d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="701c25491dcd6e28280494419172c20c" ns2:_="" ns3:_="">
     <xsd:import namespace="242e5788-3325-4b0c-8142-6fd49a4618f2"/>
@@ -1688,6 +1679,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1695,14 +1695,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95A28F03-6566-4913-9978-AC16D2197243}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8674C2BF-1067-418C-BF61-94184669BBC1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1721,6 +1713,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95A28F03-6566-4913-9978-AC16D2197243}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E19C1E25-23C7-441C-8852-7CEE76DA512D}">
   <ds:schemaRefs>

</xml_diff>